<commit_message>
Day 2 and 3 work updated
</commit_message>
<xml_diff>
--- a/Track Sheet/track Sheet.xlsx
+++ b/Track Sheet/track Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Capgemini\Track Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6078881-EA5C-47DA-AD81-3AB7EB9A65D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279B3163-E198-4AA5-B3B4-0D8778180203}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{85C9CA5B-1E92-4269-AC83-275748F848FA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>Date</t>
   </si>
@@ -112,6 +112,42 @@
   </si>
   <si>
     <t>https://github.com/wake8/freshersbatch-jan21</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MongoDB </t>
+  </si>
+  <si>
+    <t>Learned MongoDB first and second module</t>
+  </si>
+  <si>
+    <t>practicing</t>
+  </si>
+  <si>
+    <t>installation and working with mongoDB</t>
+  </si>
+  <si>
+    <t>MongoDB atlas and compass installations and basic commands on CRUD operations</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>MongoDB 2,3 modules completed</t>
+  </si>
+  <si>
+    <t>Third and fourth modules of mongoDB completed, indexing, aggregation functions,stages in aggregation,accumulator operators, and unary operators.</t>
+  </si>
+  <si>
+    <t>MongoDb robo 3T, shell</t>
+  </si>
+  <si>
+    <t>practiced the flow along with the videos</t>
+  </si>
+  <si>
+    <t>practiced in shell and after that using community edition robo 3t GUI, completed the operations shown in videos, demo data was supplied by the tuitor in his video description.</t>
   </si>
 </sst>
 </file>
@@ -179,7 +215,10 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -226,11 +265,11 @@
     <tableColumn id="1" xr3:uid="{EE4BED0B-DA3B-4521-B9D1-C3256EF6CA94}" name="Date"/>
     <tableColumn id="2" xr3:uid="{5F43B3EC-ACF0-424C-8B2F-3DA3AF55BAF8}" name="Day"/>
     <tableColumn id="3" xr3:uid="{912459BF-2D7C-4D51-A376-D23303ED9E58}" name="Hours"/>
-    <tableColumn id="4" xr3:uid="{91E98FF6-40CC-4533-B86C-6EFD7A926717}" name="Activity"/>
-    <tableColumn id="5" xr3:uid="{02C791EE-876B-4473-9A95-23DC350724E7}" name="Description" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{89CB00DF-6236-4854-A63E-0EDE7EAED563}" name="Detailed Description" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{A46DE75D-E1A4-4210-AA36-3CAF7E25E530}" name="Github Links" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{FFE1B2ED-4826-4F53-BE1F-A3FBB5CCBFE0}" name="Review Comments from mentor" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{91E98FF6-40CC-4533-B86C-6EFD7A926717}" name="Activity" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{02C791EE-876B-4473-9A95-23DC350724E7}" name="Description" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{89CB00DF-6236-4854-A63E-0EDE7EAED563}" name="Detailed Description" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{A46DE75D-E1A4-4210-AA36-3CAF7E25E530}" name="Github Links" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{FFE1B2ED-4826-4F53-BE1F-A3FBB5CCBFE0}" name="Review Comments from mentor" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -533,16 +572,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4271242B-D76C-4F54-822D-1312847D1BE0}">
-  <dimension ref="B2:I7"/>
+  <dimension ref="B2:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="4" width="11" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="3" customWidth="1"/>
     <col min="6" max="6" width="28.85546875" style="2" customWidth="1"/>
     <col min="7" max="7" width="34.7109375" style="3" customWidth="1"/>
     <col min="8" max="8" width="23" style="3" customWidth="1"/>
@@ -559,7 +598,7 @@
       <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
@@ -585,7 +624,7 @@
       <c r="D3">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
@@ -599,7 +638,7 @@
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -622,7 +661,7 @@
       <c r="D5">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -636,7 +675,7 @@
       <c r="D6">
         <v>1</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -650,7 +689,7 @@
       <c r="D7">
         <v>4</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -661,6 +700,74 @@
       </c>
       <c r="H7" s="4" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>44207</v>
+      </c>
+      <c r="C8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>44208</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="D11">
+        <v>3</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>